<commit_message>
[dattt] update size column for Template PT and PTTT
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplatePT.xlsx
+++ b/ATV_Allowance/Templates/TemplatePT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>Đài Phát thanh - Truyền hình An Giang</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Trừ chỉ tiêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -107,21 +110,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -288,7 +291,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -331,14 +334,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -347,18 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,135 +678,135 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="7.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="21" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.75" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.25" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.75" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="16.75" style="21" customWidth="1"/>
+    <col min="20" max="20" width="11.25" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:20" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26" t="s">
+      <c r="M3" s="23"/>
+      <c r="N3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="22" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="26" t="s">
+      <c r="Q3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="28" t="s">
+      <c r="S3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="T3" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
@@ -840,11 +843,291 @@
       <c r="O4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="26"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="23"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="10"/>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7" s="20"/>
+      <c r="T7" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T8" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="P3:P4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="66" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.75" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.75" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.25" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.25" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.75" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="16.75" style="21" customWidth="1"/>
+    <col min="20" max="20" width="11.25" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+    </row>
+    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+    </row>
+    <row r="3" spans="1:20" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="23"/>
+      <c r="P3" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="23"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
@@ -870,10 +1153,10 @@
     </row>
     <row r="6" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -892,285 +1175,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S7" s="20"/>
-      <c r="T7" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="T8" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="S3:S4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:T12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="7.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="21" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-    </row>
-    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-    </row>
-    <row r="3" spans="1:20" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="S3" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="26"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="10"/>
-    </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S7" s="20"/>
       <c r="T7" s="13" t="s">
         <v>16</v>
@@ -1219,6 +1224,6 @@
     <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="66" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[dattt] add template PT and PTTT (pixel from user pc)
</commit_message>
<xml_diff>
--- a/ATV_Allowance/Templates/TemplatePT.xlsx
+++ b/ATV_Allowance/Templates/TemplatePT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\job\ATV-Allowance\ATV-Allowance\ATV_Allowance\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="PV" sheetId="1" r:id="rId1"/>
@@ -108,10 +103,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -291,7 +286,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -328,51 +323,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -688,136 +683,136 @@
   </sheetPr>
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="7.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="16" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="5.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.21875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.21875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.33203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-    </row>
-    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-    </row>
-    <row r="3" spans="1:20" s="7" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+    </row>
+    <row r="3" spans="1:20" s="7" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="21" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+    <row r="4" spans="1:20" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
@@ -854,13 +849,13 @@
       <c r="O4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="18"/>
-    </row>
-    <row r="5" spans="1:20" s="23" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="26"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+    </row>
+    <row r="5" spans="1:20" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
         <v>25</v>
@@ -884,42 +879,42 @@
       <c r="S5" s="14"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" s="23" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:20" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="29"/>
-    </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="S7" s="15"/>
       <c r="T7" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
@@ -933,11 +928,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A1:T1"/>
@@ -952,9 +950,6 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -968,136 +963,136 @@
   </sheetPr>
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="7.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="16" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="5.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="4.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.21875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="4.21875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.33203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="16" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-    </row>
-    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-    </row>
-    <row r="3" spans="1:20" s="7" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+    </row>
+    <row r="3" spans="1:20" s="7" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18" t="s">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="21" t="s">
+      <c r="O3" s="24"/>
+      <c r="P3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+    <row r="4" spans="1:20" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
@@ -1134,13 +1129,13 @@
       <c r="O4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="18"/>
-    </row>
-    <row r="5" spans="1:20" s="23" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="26"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+    </row>
+    <row r="5" spans="1:20" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1162,42 +1157,42 @@
       <c r="S5" s="14"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" s="23" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:20" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="29"/>
-    </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="27"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" spans="1:20" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="S7" s="15"/>
       <c r="T7" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="T8" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
@@ -1211,11 +1206,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="A1:T1"/>
@@ -1228,11 +1228,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>